<commit_message>
Update competitive audit & report for project
</commit_message>
<xml_diff>
--- a/02-ux-design-process/Week4: Ideation/Competitive-audit/Project-portfolio/Competitor-audit-Animal-Shelter.xlsx
+++ b/02-ux-design-process/Week4: Ideation/Competitive-audit/Project-portfolio/Competitor-audit-Animal-Shelter.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t xml:space="preserve">Competitive audit
 </t>
@@ -140,31 +140,31 @@
     <t xml:space="preserve">Descriptiveness</t>
   </si>
   <si>
-    <t xml:space="preserve">Adopt Me</t>
+    <t xml:space="preserve">Petfinder</t>
   </si>
   <si>
     <t xml:space="preserve">Direct</t>
   </si>
   <si>
-    <t xml:space="preserve">Kansas City, MO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 types of burgers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$$$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.BurgerNest.com</t>
+    <t xml:space="preserve">North America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pets of all sizes and breeds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.petfinder.com</t>
   </si>
   <si>
     <t xml:space="preserve">Small</t>
   </si>
   <si>
-    <t xml:space="preserve">Families</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Traditional American-style food</t>
+    <t xml:space="preserve">All lovers of pets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connecting animals and people through searchable database</t>
   </si>
   <si>
     <r>
@@ -214,39 +214,41 @@
       </rPr>
       <t xml:space="preserve">+ Fully responsive
 + Animations added to enhance the mobile experience 
-- Menu is hard to read</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
++ Mobile app is available</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Okay
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
+      <t xml:space="preserve">Good
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+ "Create account" feature
-- Users have to download PDF of menu to open it </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
++ Can save search result
+- No favorites
+- No video of pet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
@@ -257,89 +259,89 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Website only available in English
-- Menu is included as an image and is hard to read </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Okay
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Easy to find the menu
-- Needed to search to find hours
-- Home page is too busy</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Okay
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Somewhat difficult to navigate 
-- Some elements seem clickable but are not</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Needs work
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- No brand identity at all</t>
+ </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Good
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Easy to find the navigation menu
++ Easy to find key info
+- Pet list page is too busy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Outstanding
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Very easy to navigate 
++ Familiar way to navigate (e.g., arrow icons)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Outstanding
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Strong brand identity, including colors, font, style, motion, imagery, and photography</t>
     </r>
   </si>
   <si>
@@ -355,35 +357,41 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Okay
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ All key info is present
-- Unnecessary details </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Petfinder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 types of burgers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.TheSpottyCow.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Local millennials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fun and friendly branding </t>
+      <t xml:space="preserve">Outstanding 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Easy to follow 
++ Short and to the point</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Adopt a Pet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New York, US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dogs and cats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$$$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.adoptapet.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential adopters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adopt and rehome pets of different sizes and breeds</t>
   </si>
   <si>
     <r>
@@ -433,42 +441,42 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+ Fully responsive 
-+ Engaging animations (same as desktop) 
-+ App can be downloaded to collect points</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
++ Engaging animations (same as desktop)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Outstanding
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
+      <t xml:space="preserve">Good
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+ "Create account" feature
-+ Store locator feature
-+ Online ordering feature with pickup/delivery options
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
++ Can save search result
+- No favorites
+- No video of pet
+- </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
@@ -479,7 +487,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
@@ -511,7 +519,9 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+ Fun to use
-- Difficult to find key info (menu, location, hours) due to animation load time  </t>
++ Easy to find key info
+- Home page is cluttered with images
+- Difficult to find key info due to animation load time  </t>
     </r>
   </si>
   <si>
@@ -540,30 +550,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Outstanding
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Strong brand identity, including colors, font, style, motion, imagery, and photography</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Fun and indirect</t>
   </si>
   <si>
@@ -591,31 +577,25 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Pawslikeme</t>
+    <t xml:space="preserve">Rescue Me</t>
   </si>
   <si>
     <t xml:space="preserve">Indirect</t>
   </si>
   <si>
-    <t xml:space="preserve">Kansas City, MO
-Chicago, IL
-St Louis, MO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 types of burgers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.BeefEatersFoodTruck.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">College students </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family owned and operated, 
-with a devoted customer following </t>
+    <t xml:space="preserve">Pennsylvania Ave. NW, #2001 Washington, DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pets of different breeds and sizes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.rescueme.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Families</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rescue Me helps dogs, cats, horses, birds, and other animals find homes.</t>
   </si>
   <si>
     <r>
@@ -652,26 +632,26 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Okay
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Key information is present
-- Not fully responsive</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
+      <t xml:space="preserve">Needs work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Navigation is hard to read
+- Not responsive</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
@@ -682,40 +662,42 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">- Users have to download PDF of menu to open it 
-- Checkout process requires user to input payment info twice</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
+      <t xml:space="preserve">+ Search by breed
+- No favorites
+- No video of pet
+- No user sign up feature</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Okay
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
+      <t xml:space="preserve">Needs work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="&quot;Google Sans&quot;, Arial"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">+ Website available in two languages
-- Menu isn't compatible with screen reader technologies 
-- Menu is included as an image and is hard to read </t>
+      <t xml:space="preserve">- Website only available in English
+- Navigation menu isn't compatible with screen reader technologies 
+- Navigation menu is included as an image and is hard to read </t>
     </r>
   </si>
   <si>
@@ -739,7 +721,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">+ Easy to find key info (menu, location, hours) 
+      <t xml:space="preserve">+ Easy to find key info 
 + Info is kept up to date (e.g., holiday opening)</t>
     </r>
   </si>
@@ -753,19 +735,20 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Outstanding 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Very easy to navigate 
-+ Familiar way to navigate (e.g., swipe)</t>
+      <t xml:space="preserve">Needs Work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Somewhat difficult to navigate 
+- Some links are not clickable
+- Unfamiliar way to navigate</t>
     </r>
   </si>
   <si>
@@ -803,220 +786,19 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Outstanding 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Easy to follow 
-+ Short and to the point</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">The Vegan Cow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Various - international</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 types of burgers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.TheVeganCow.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vegans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specialty vegan burgers</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Outstanding 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Visually appealing imagery
-+ Clean design</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Outstanding 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Fully responsive 
-+ Menu is easy to read</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="&quot;Google Sans&quot;, Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Outstanding
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="&quot;Google Sans&quot;, Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Store locator feature
-+ Website features a nutrition calculator
-+  "Trending" menu</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="&quot;Google Sans&quot;, Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Outstanding
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="&quot;Google Sans&quot;, Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Website available in six languages
-+ Menu is compatible with screen reader technologies
-+ Images of menu items are clear and legible</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Good
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Easy to find key info (menu, location, hours) 
-- Seasonal and holiday times are not clear </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Outstanding
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Easy to navigate
-+ Easy to switch locations and languages</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Serious and direct</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Outstanding 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Google Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Short
-+ Focused on info relevant to target audience</t>
+      <t xml:space="preserve">Okay
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Google Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ All key info is present
+- Unnecessary details </t>
     </r>
   </si>
 </sst>
@@ -1084,7 +866,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;Google Sans&quot;"/>
       <family val="0"/>
@@ -1106,14 +888,14 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;Google Sans&quot;, Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;Google Sans&quot;, Arial"/>
       <family val="0"/>
@@ -1213,7 +995,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1259,26 +1041,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thick">
-        <color rgb="FF4285F4"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FF4285F4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FF4285F4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1305,7 +1067,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1424,42 +1186,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="14" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1549,10 +1275,10 @@
   </sheetPr>
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B5" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="topRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1701,7 +1427,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
         <v>25</v>
       </c>
@@ -1757,7 +1483,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
@@ -1765,69 +1491,69 @@
         <v>26</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G6" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M6" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="P6" s="29" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="R6" s="27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>62</v>
@@ -1869,80 +1595,25 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="K8" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="M8" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="N8" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="O8" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="P8" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q8" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="R8" s="38" t="s">
-        <v>87</v>
-      </c>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="7">
@@ -1954,6 +1625,10 @@
     <mergeCell ref="L3:O3"/>
     <mergeCell ref="Q3:R3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F5" r:id="rId1" display="www.petfinder.com"/>
+    <hyperlink ref="F7" r:id="rId2" display="www.rescueme.org"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Add examples of competitive audit & report
</commit_message>
<xml_diff>
--- a/02-ux-design-process/Week4: Ideation/Competitive-audit/Project-portfolio/Competitor-audit-Animal-Shelter.xlsx
+++ b/02-ux-design-process/Week4: Ideation/Competitive-audit/Project-portfolio/Competitor-audit-Animal-Shelter.xlsx
@@ -45,7 +45,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Compare the user experience of each competitor's website</t>
+      <t xml:space="preserve">Compare the user experience of each competitor's app</t>
     </r>
   </si>
   <si>
@@ -494,7 +494,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Website only available in English
-- Menu isn't compatible with screen reader technologies </t>
+- Navigation menu isn't compatible with screen reader technologies </t>
     </r>
   </si>
   <si>
@@ -1276,9 +1276,9 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N5" activeCellId="0" sqref="N5"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1297,7 +1297,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add screenshots of info about goal statement
</commit_message>
<xml_diff>
--- a/02-ux-design-process/Week4: Ideation/Competitive-audit/Project-portfolio/Competitor-audit-Animal-Shelter.xlsx
+++ b/02-ux-design-process/Week4: Ideation/Competitive-audit/Project-portfolio/Competitor-audit-Animal-Shelter.xlsx
@@ -1278,7 +1278,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1631,7 +1631,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>